<commit_message>
update for review v3
</commit_message>
<xml_diff>
--- a/data/FPGA list.xlsx
+++ b/data/FPGA list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNN硬件\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\tex\TRETS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="240">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -588,226 +587,361 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>三维卷积加速器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xeon+FPGA实现1比特NN和1比特权重两种</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在FPGA上加速RCNN；自动映射方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用PVT-margin提升频率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用一个DSP做两个低比特乘累加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2比特NN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对比了不同平台上运行一个优化版本的GRU的性能，FPGA超过CPU和GPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给不同层分配不同展开系数的硬件，提升利用率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用嵌套余数系来表示数，简化MAC单元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>222.1G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.96W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多层流水线形式的自动硬件映射；16bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对比了不同平台上运行BNN的性能，FPGA超过CPU和GPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Caffe到SDAccel；winograd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用RAM查表实现1bit操作，实现1比特NN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuse layer；winograd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于硬件单元库的自动映射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSTM加速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An OpenCL Deep Learning Accelerator on Arria 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chi Zhang and Viktor Prasanna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abhinav Podili, Chi Zhang and Viktor Prasanna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatic Code Generation of Convolutional Neural Networks in FPGA Implementation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhiqiang Liu, Yong Dou, Jingfei Jiang, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong Nguyen, Daewoo Kim and Jongeun Lee </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Atul Rahman, Sangyun Oh, Jongeun Lee, et al. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shreejith Shanker, Bezborah Anshuman and Suhaib A. Fahmy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Atul Rahman, Jongeun Lee and Kiyoung Choi </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Caffeine: Towards Uniformed Representation and Acceleration for Deep Convolutional Neural Networks </t>
+  </si>
+  <si>
+    <t>Chen Zhang, Zhenman Fang, Peipei Zhou, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICCAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于HLS的自动化映射工具；设计空间搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Double MAC: Doubling the Performance of Convolutional Neural Networks on Modern FPGAs </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个DSP做两个乘法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Design Space Exploration of FPGA Accelerators for Convolutional Neural Networks </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计空间搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCELERATED ARTIFICIAL NEURAL NETWORKS ON FPGA FOR FAULT DETECTION IN AUTOMOTIVE SYSTEMS </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在检错系统中的应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">EFFICIENT FPGA ACCELERATION OF CONVOLUTIONAL NEURAL NETWORKS USING LOGICAL-3D COMPUTE ARRAY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scalable High-Performance Architecture for Convolutional Ternary Neural Networks on FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fast and Efficient Implementation of Convolutional Neural Networks on FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Caffeinated FPGAs: FPGA Framework For Convolutional Neural Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Deep Convolutional Neural Network using Nested Residue Number System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customizing Neural Networks for Efficient FPGA Implementation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Energy-Efficient CNN Implementation on a Deeply Pipelined FPGA Cluster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用systolic array提高系统时钟频率；研究了阵列配置的选择优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计了一种展开方式，以及参数选取方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选取合适的batch size来优化带宽需求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Escher: A CNN Accelerator with Flexible Buffering to Minimize Off-Chip Transfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High-Performance Video Content Recognition with Long-term Recurrent Convolutional Network for FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESE: Efficient Speech Recognition Engine with Sparse LSTM on FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fpgaConvNet: Automated Mapping of Convolutional Neural Networks on FPGAs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frequency Domain Acceleration of Convolutional Neural Networks on CPU-FPGA Shared Memory System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploring Heterogeneous Algorithms for Accelerating Deep Convolutional Neural Networks on FPGAs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FP-DNN: An Automated Framework for Mapping Deep Neural Networks onto FPGAs with RTL-HLS Hybrid Templates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLINK: Compact LSTM Inference Kernel for Energy Efficient Neuro feedback Devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhe Chen, Andrew Howe, Hugh T. Blair, and Jason Cong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Fully Onchip Binarized Convolutional Neural Network FPGA Impelmentation with Accurate Inference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Li Yang, Zhezhi Hem Deliang Fan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCP: Layer Clusters Paralleling Mapping Mechanism for Accelerating Inception and Residual Networks on FPGA</t>
+  </si>
+  <si>
+    <t>Xinhan Lin, Shouyi Yin, fengbin Tu, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FlexiGAN: An End-to-End Solution for FPGA Acceleration of Generative Adversarial Networks</t>
+  </si>
+  <si>
     <t>F-C3D: FPGA-based 3-Dimensional Convolutional Neural Network</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>三维卷积加速器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xeon+FPGA实现1比特NN和1比特权重两种</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在FPGA上加速RCNN；自动映射方案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>利用PVT-margin提升频率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>利用一个DSP做两个低比特乘累加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2比特NN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对比了不同平台上运行一个优化版本的GRU的性能，FPGA超过CPU和GPU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>给不同层分配不同展开系数的硬件，提升利用率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用嵌套余数系来表示数，简化MAC单元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>222.1G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8.96W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多层流水线形式的自动硬件映射；16bit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对比了不同平台上运行BNN的性能，FPGA超过CPU和GPU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Caffe到SDAccel；winograd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用RAM查表实现1bit操作，实现1比特NN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuse layer；winograd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基于硬件单元库的自动映射</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSTM加速</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>An OpenCL Deep Learning Accelerator on Arria 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chi Zhang and Viktor Prasanna</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abhinav Podili, Chi Zhang and Viktor Prasanna</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automatic Code Generation of Convolutional Neural Networks in FPGA Implementation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zhiqiang Liu, Yong Dou, Jingfei Jiang, et al.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Dong Nguyen, Daewoo Kim and Jongeun Lee </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Atul Rahman, Sangyun Oh, Jongeun Lee, et al. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shreejith Shanker, Bezborah Anshuman and Suhaib A. Fahmy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Atul Rahman, Jongeun Lee and Kiyoung Choi </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Caffeine: Towards Uniformed Representation and Acceleration for Deep Convolutional Neural Networks </t>
-  </si>
-  <si>
-    <t>Chen Zhang, Zhenman Fang, Peipei Zhou, et al.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICCAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基于HLS的自动化映射工具；设计空间搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Double MAC: Doubling the Performance of Convolutional Neural Networks on Modern FPGAs </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一个DSP做两个乘法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Design Space Exploration of FPGA Accelerators for Convolutional Neural Networks </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计空间搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCELERATED ARTIFICIAL NEURAL NETWORKS ON FPGA FOR FAULT DETECTION IN AUTOMOTIVE SYSTEMS </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在检错系统中的应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">EFFICIENT FPGA ACCELERATION OF CONVOLUTIONAL NEURAL NETWORKS USING LOGICAL-3D COMPUTE ARRAY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scalable High-Performance Architecture for Convolutional Ternary Neural Networks on FPGA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fast and Efficient Implementation of Convolutional Neural Networks on FPGA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Caffeinated FPGAs: FPGA Framework For Convolutional Neural Networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Deep Convolutional Neural Network using Nested Residue Number System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customizing Neural Networks for Efficient FPGA Implementation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Energy-Efficient CNN Implementation on a Deeply Pipelined FPGA Cluster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用systolic array提高系统时钟频率；研究了阵列配置的选择优化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计了一种展开方式，以及参数选取方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选取合适的batch size来优化带宽需求</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Escher: A CNN Accelerator with Flexible Buffering to Minimize Off-Chip Transfer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>High-Performance Video Content Recognition with Long-term Recurrent Convolutional Network for FPGA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESE: Efficient Speech Recognition Engine with Sparse LSTM on FPGA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fpgaConvNet: Automated Mapping of Convolutional Neural Networks on FPGAs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Frequency Domain Acceleration of Convolutional Neural Networks on CPU-FPGA Shared Memory System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exploring Heterogeneous Algorithms for Accelerating Deep Convolutional Neural Networks on FPGAs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FP-DNN: An Automated Framework for Mapping Deep Neural Networks onto FPGAs with RTL-HLS Hybrid Templates</t>
+    <t>ReBNet: Residual Binarized Neural Network</t>
+  </si>
+  <si>
+    <t>Exploration of Low Numeric Precision Deep Learning Inference Using Intel FPGAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPDeep: Acceleration and Load Balancing of CNN Training on FPGA Clusters </t>
+  </si>
+  <si>
+    <t>PQ-CNN: Accelerating Product Quantized Convolutional Neural Network on FPGA</t>
+  </si>
+  <si>
+    <t>AccDNN: an IP-based DNN Generator for FPGAs</t>
+  </si>
+  <si>
+    <t>Accelerator Design with Effective Resource Utilization for Binary Convolutional Neural Networks on an FPGA</t>
+  </si>
+  <si>
+    <t>A PYNQ-based Framework for Rapid CNN Prototyping</t>
+  </si>
+  <si>
+    <t>A FPGA friendly approximate computing framework with hybrid Neural networks</t>
+  </si>
+  <si>
+    <t>In-Package Domain-Specific ASICs for Intel® Stratix® 10 FPGAs: A Case Study of Accelerating Deep Learning Using TensorTile ASIC</t>
+  </si>
+  <si>
+    <t>FPGA-based LSTM Acceleration for Real-Time EEG Signal Processing</t>
+  </si>
+  <si>
+    <t>Mapping Large-Scale DNNs on Asymmetric FPGAs</t>
+  </si>
+  <si>
+    <t>Software-Defined FPGA-Based Accelerator for Deep Convolutional Neural Networks</t>
+  </si>
+  <si>
+    <t>A Low-Power Deconvolutional Accelerator for Convolutional Neural Network Based Segmentation on FPGA</t>
+  </si>
+  <si>
+    <t>Exploration of Low Numeric Precision Deep Learning Inference Using Intel® FPGAs</t>
+  </si>
+  <si>
+    <t>A Self-adaptation Method of Fitting Convolutional Neural Network into FPGA</t>
+  </si>
+  <si>
+    <t>A Framework for Generating High Throughput CNN Implementations on FPGAs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatic Optimising CNN with Depthwise Separable Convolution on FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ruizhe Zhao, Xinyu Niu, Wayne Luk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haiyue Song, Xiang Song, Tianjian Li, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhe Chen, Andrew Howe, Hugh T. Bair, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ning Mao, Zhihong Huang, Xing Wei, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duncan Moss, Srivatsan Krishnan, Eriko Nurvitadhi, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eriko Nurvitadhi, Jeff Cook, Asit Mishra, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wentai Zhang, Jiaxi Zhang, Minghua Shen, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yankang Du, Qinrang Liu, Shuai Wei, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuanglong Liu, Xinyu Niu, Wayne Luk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Philip Colangelo, Nasibeh Nasiri, Eriko Nurvitadhi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Towards a Uniform Template-based Architecture for Accelerating 2D and 3D CNNs on FPGA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Junzhong Shen, Yaou Huang, Zelong Wang, et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Customizable Matrix Multiplication Framework for the Intel HARPv2 Xeon+FPGA Platform - A Deep Learning Case Study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hanqing Zeng, Ren Chen, Chi Zhang, et al.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -927,7 +1061,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -957,6 +1091,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1330,7 +1473,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -1353,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -1387,7 +1530,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>46</v>
@@ -1404,10 +1547,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="1">
         <v>2017</v>
@@ -1514,902 +1657,1170 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D18" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D30" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D31" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G22">
-        <v>8.0399999999999991</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>7</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>10</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>11</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>12</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D32" s="1">
         <v>2017</v>
       </c>
-      <c r="E32" t="s">
-        <v>113</v>
+      <c r="E32" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1">
         <v>2017</v>
       </c>
-      <c r="E33" t="s">
-        <v>145</v>
+      <c r="E33" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="D34" s="1">
         <v>2017</v>
       </c>
-      <c r="E34" t="s">
-        <v>147</v>
+      <c r="E34" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34">
+        <v>8.0399999999999991</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1">
         <v>2017</v>
       </c>
-      <c r="E35" t="s">
-        <v>148</v>
+      <c r="E35" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>196</v>
+        <v>130</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1">
         <v>2017</v>
       </c>
-      <c r="E36" t="s">
-        <v>149</v>
+      <c r="E36" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D39" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D40" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>12</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E41" t="s">
-        <v>89</v>
-      </c>
+        <v>2018</v>
+      </c>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>13</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E42" t="s">
-        <v>153</v>
-      </c>
+        <v>2018</v>
+      </c>
+      <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>14</v>
-      </c>
+      <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="C43" s="1"/>
       <c r="D43" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E43" t="s">
-        <v>154</v>
-      </c>
+        <v>2018</v>
+      </c>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>15</v>
-      </c>
+      <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E44" t="s">
-        <v>155</v>
-      </c>
+        <v>2018</v>
+      </c>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D46" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E46" t="s">
-        <v>158</v>
-      </c>
-      <c r="F46" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>2</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E47" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>3</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>4</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+      <c r="B50" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E50" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D51" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E51" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="1">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E52" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D53" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="1">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E54" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" t="s">
-        <v>83</v>
+        <v>69</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D55" s="1">
         <v>2017</v>
       </c>
       <c r="E55" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>2</v>
-      </c>
-      <c r="B56" t="s">
-        <v>200</v>
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D56" s="1">
         <v>2017</v>
       </c>
       <c r="E56" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D57" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E57" t="s">
-        <v>163</v>
+        <v>2017</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
+      <c r="A58" s="1">
+        <v>9</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D59" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E59" t="s">
-        <v>100</v>
+        <v>2017</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D60" s="1">
         <v>2017</v>
       </c>
-      <c r="E60" t="s">
-        <v>164</v>
+      <c r="E60" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
+      <c r="A61" s="1">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E61" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D62" s="1">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E62" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
+      <c r="A63" s="1">
+        <v>14</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E63" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
+        <v>15</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E64" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>1</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D64" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="B66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D66" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E66" t="s">
+        <v>157</v>
+      </c>
+      <c r="F66" t="s">
+        <v>155</v>
+      </c>
+      <c r="G66" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>2</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" s="1">
+      <c r="B67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="1">
         <v>2016</v>
       </c>
-      <c r="E65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="E67" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>3</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" s="5">
+      <c r="B68" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="1">
         <v>2016</v>
       </c>
-      <c r="E66" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
+      <c r="E68" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D69" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E69" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>1</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D68" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E68" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="5">
-        <v>2</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D69" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E69" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="5">
-        <v>3</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D70" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E70" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="5">
-        <v>4</v>
-      </c>
       <c r="B71" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="D71" s="1">
         <v>2016</v>
       </c>
       <c r="E71" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>1</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>1</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>199</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>3</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>1</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E82" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>2</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E83" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>1</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E85" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>1</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E87" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>2</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>3</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="5">
+        <v>2016</v>
+      </c>
+      <c r="E89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>1</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E92" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
+        <v>3</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D93" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>4</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D94" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E94" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
+        <v>1</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E96" t="s">
         <v>177</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="5">
-        <v>1</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D73" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E73" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2418,18 +2829,18 @@
     <sortCondition ref="B31:B45"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A95:D95"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A65:D65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>